<commit_message>
Implemented GetTransactionItem and Progress - only need to implement to check if the images are uploaded
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdjan.suc\Documents\UiPath\KupujemProdajemBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A29FDD2-76DF-4118-B4D4-B3829E3E3B3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06302168-53ED-4BD4-82D4-2A57351A839A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>Queue1</t>
+  </si>
+  <si>
+    <t>TransactionData</t>
+  </si>
+  <si>
+    <t>Data\TransactionData.xlsx</t>
+  </si>
+  <si>
+    <t>TransactionDataSheet</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
   </si>
 </sst>
 </file>
@@ -546,7 +558,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -631,8 +643,22 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Dodato: -Dodatna logika kako bi bolje pronalazio predmet oglasa
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srdjan.suc\Documents\UiPath\KupujemProdajemBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06302168-53ED-4BD4-82D4-2A57351A839A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E9D0616-ED3A-41A4-8179-AB0F8917A110}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -196,7 +196,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -207,12 +207,20 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,10 +244,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -558,7 +567,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -631,7 +640,7 @@
       <c r="A6" t="s">
         <v>48</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>